<commit_message>
Stage.xlsx 업뎃, PartyBall.docx 업뎃
</commit_message>
<xml_diff>
--- a/Documents/PartyBall/PartyBall'sStages.xlsx
+++ b/Documents/PartyBall/PartyBall'sStages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsh39\OneDrive\project\Jagu_Agis\Documents\PartyBall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDD6603-D6E5-4974-A63D-FDB8E76361EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104DFEFE-91E6-42F0-8756-5399527BC2EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6654ADE8-FED1-4A0B-8F79-39BD6602AA37}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>셀 경계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -61,6 +61,10 @@
   </si>
   <si>
     <t>Stage1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tutorial</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -393,24 +397,60 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -418,42 +458,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -615,13 +619,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>33129</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>33130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>216009</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>216010</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -683,13 +687,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>23854</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>36111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>214354</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>226611</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -751,13 +755,13 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>33129</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>19879</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>216009</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>202759</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -819,13 +823,13 @@
     <xdr:from>
       <xdr:col>27</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>29484</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>219984</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -842,6 +846,142 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6649941" y="1222180"/>
+          <a:ext cx="190500" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>33129</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>33130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>216009</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>216010</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="타원 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF169E27-F9DC-440B-BCF2-459DB73C1B96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4446103" y="1702904"/>
+          <a:ext cx="182880" cy="182880"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>23854</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>36111</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>214354</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>226611</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="사각형: 둥근 모서리 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8A39776-1FCF-4C1B-95F4-689D3FAEC7BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5417489" y="4091276"/>
           <a:ext cx="190500" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -1183,235 +1323,324 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F014CC21-94BA-4A4A-B0AC-D9B5269E619A}">
-  <dimension ref="B1:AG10"/>
+  <dimension ref="B1:AG20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.19921875" defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="2:33" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:33" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-      <c r="I2" s="3" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="I2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="23" t="s">
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="20"/>
+    </row>
+    <row r="3" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="20"/>
+    </row>
+    <row r="4" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="3"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="4"/>
+      <c r="I4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="20"/>
+    </row>
+    <row r="5" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="4"/>
+      <c r="I5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="8"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="20"/>
+    </row>
+    <row r="6" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="3"/>
+      <c r="D6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="4"/>
+      <c r="I6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="8"/>
+      <c r="V6" s="2"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="20"/>
+    </row>
+    <row r="7" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="3"/>
+      <c r="D7" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="4"/>
+      <c r="I7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="8"/>
+      <c r="T7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="20"/>
+    </row>
+    <row r="8" spans="2:33" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="I8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="8"/>
+      <c r="T8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="20"/>
+    </row>
+    <row r="9" spans="2:33" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="1"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="20"/>
+    </row>
+    <row r="10" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+    </row>
+    <row r="12" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q12" s="20"/>
+      <c r="R12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23"/>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="23"/>
-      <c r="AG2" s="3"/>
-    </row>
-    <row r="3" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="13"/>
-      <c r="AC3" s="13"/>
-      <c r="AD3" s="13"/>
-      <c r="AE3" s="13"/>
-      <c r="AF3" s="13"/>
-      <c r="AG3" s="3"/>
-    </row>
-    <row r="4" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="4"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="5"/>
-      <c r="I4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Z4" s="12"/>
-      <c r="AF4" s="12"/>
-      <c r="AG4" s="3"/>
-    </row>
-    <row r="5" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="4"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="5"/>
-      <c r="I5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="X5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
-      <c r="AD5" s="2"/>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="3"/>
-    </row>
-    <row r="6" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="4"/>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="5"/>
-      <c r="I6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="3"/>
-    </row>
-    <row r="7" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="4"/>
-      <c r="D7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="5"/>
-      <c r="I7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Z7" s="12"/>
-      <c r="AB7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AF7" s="12"/>
-      <c r="AG7" s="3"/>
-    </row>
-    <row r="8" spans="2:33" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="I8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Z8" s="12"/>
-      <c r="AF8" s="12"/>
-      <c r="AG8" s="3"/>
-    </row>
-    <row r="9" spans="2:33" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="1"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="1"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="13"/>
-      <c r="AD9" s="13"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="3"/>
-    </row>
-    <row r="10" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
-      <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="19"/>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="19"/>
+      <c r="AE12" s="19"/>
+      <c r="AF12" s="19"/>
+      <c r="AG12" s="20"/>
+    </row>
+    <row r="13" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q13" s="20"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="20"/>
+    </row>
+    <row r="14" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q14" s="20"/>
+      <c r="R14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="20"/>
+    </row>
+    <row r="15" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q15" s="20"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="X15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AF15" s="8"/>
+      <c r="AG15" s="20"/>
+    </row>
+    <row r="16" spans="2:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q16" s="20"/>
+      <c r="R16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="20"/>
+    </row>
+    <row r="17" spans="17:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q17" s="20"/>
+      <c r="R17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Z17" s="8"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AF17" s="8"/>
+      <c r="AG17" s="20"/>
+    </row>
+    <row r="18" spans="17:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q18" s="20"/>
+      <c r="R18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Z18" s="8"/>
+      <c r="AF18" s="8"/>
+      <c r="AG18" s="20"/>
+    </row>
+    <row r="19" spans="17:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q19" s="20"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="1"/>
+      <c r="Z19" s="12"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="20"/>
+    </row>
+    <row r="20" spans="17:33" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="20"/>
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="20"/>
+      <c r="AB20" s="20"/>
+      <c r="AC20" s="20"/>
+      <c r="AD20" s="20"/>
+      <c r="AE20" s="20"/>
+      <c r="AF20" s="20"/>
+      <c r="AG20" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="R2:AF2"/>
-    <mergeCell ref="R10:AF10"/>
-    <mergeCell ref="AG2:AG10"/>
+  <mergeCells count="14">
     <mergeCell ref="Q2:Q10"/>
+    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="Y2:Y10"/>
+    <mergeCell ref="R10:X10"/>
+    <mergeCell ref="R12:AF12"/>
+    <mergeCell ref="R20:AF20"/>
+    <mergeCell ref="AG12:AG20"/>
+    <mergeCell ref="Q12:Q20"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D6:F6"/>

</xml_diff>